<commit_message>
Updated for EA 23.229 Stable. Added two action safety modes (before action / during action). Improved threshold protections with priorities: Stamina Value, Stamina Phase, HP, Mana.
EA 23.229 Stable に対応しました。アクション開始前 / アクション中の 2 種類の安全モードを追加しました。しきい値保護を強化し、スタミナ数値・スタミナフェーズ・HP・マナの優先度を導入しました。

现已更新至 EA 23.229 Stable。新增动作前 / 动作中的两种安全模式。改进了阈值保护并加入优先级：体力数值、体力阶段、生命值、法力值。
</commit_message>
<xml_diff>
--- a/translations.xlsx
+++ b/translations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -109,13 +109,61 @@
     <t xml:space="preserve">topic01</t>
   </si>
   <si>
-    <t xml:space="preserve">Stamina Threshold Value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">スタミナしきい値の数値</t>
-  </si>
-  <si>
-    <t xml:space="preserve">耐力阈值数值</t>
+    <t xml:space="preserve">Stamina Threshold Value (Priority 1)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">スタミナしきい値の数値（優先度</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">耐力阈值数值（优先级</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">）</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">topic02</t>
@@ -133,13 +181,61 @@
     <t xml:space="preserve">topic03</t>
   </si>
   <si>
-    <t xml:space="preserve">Stamina Threshold Phase</t>
-  </si>
-  <si>
-    <t xml:space="preserve">スタミナしきい値のフェーズ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">耐力阈值阶段</t>
+    <t xml:space="preserve">Stamina Threshold Phase (Priority 2)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">スタミナしきい値のフェーズ（優先度</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">耐力阈值阶段（优先级</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">）</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">dropdown.item01</t>
@@ -164,6 +260,381 @@
   </si>
   <si>
     <t xml:space="preserve">过劳</t>
+  </si>
+  <si>
+    <t xml:space="preserve">title01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">General (Required, choose 1)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">一般（必須、いずれか</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">つ）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">常规（必选，仅选</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">个）</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable Pre-Action Check</t>
+  </si>
+  <si>
+    <t xml:space="preserve">スタミナ開始前チェックを有効にする</t>
+  </si>
+  <si>
+    <t xml:space="preserve">启用动作前体力检查</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tooltip01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stop actions before they start when stamina is low. Recommended for permadeath or hardcore play. May stop some actions that do not consume stamina.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">スタミナが低いと、アクション開始前に行動を停止します。ハードコアや永久死プレイに推奨。スタミナを消費しない行動も停止される場合があります。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">体力过低时在动作开始前停止行动。适用于硬核或永久死亡模式。某些不消耗体力的动作也可能会被停止。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable Stamina Check</t>
+  </si>
+  <si>
+    <t xml:space="preserve">スタミナ低下チェックを有効にする</t>
+  </si>
+  <si>
+    <t xml:space="preserve">启用体力消耗检查</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tooltip02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stop actions when stamina drops during the action.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">行動中にスタミナが低下した場合、行動を停止します。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">在行动过程中体力下降到阈值以下时停止行动。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">topic04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HP Threshold Value (Priority 3)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">HP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">しきい値（優先度</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">生命值阈值（优先级</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">）</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable HP Threshold Value</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">HP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">のしきい値を有効にします</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">启用生命值阈值选项</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tooltip03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The HP threshold value at which actions will be stopped. Triggered when stamina drops below zero and begins damaging HP.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">HP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">の閾値。この値を下回るとスタミナがマイナスになった際に</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">HP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ダメージが始まり、行動が停止します。</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">生命值阈值。耐力降至负数开始扣除生命值时，当生命值低于该值将停止行动。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">topic05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mana Threshold Value (Priority 4)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">マナしきい値（優先度</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">法力值阈值（优先级</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">）</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable Mana Threshold Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">マナのしきい値を有効にします</t>
+  </si>
+  <si>
+    <t xml:space="preserve">启用法力值阈值选项</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tooltip04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The mana threshold value at which actions will be stopped. Triggered when stamina and HP drop below zero and starts damaging mana. Useful when using the Mana Body feat.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">マナの閾値。この値を下回ると、スタミナと</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">HP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">が</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">未満になり、疲労ダメージがマナに対して発生した際に行動が停止します。「マナの体」特性を使用している場合に有効です。</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">法力值阈值。当耐力与生命值降至零以下并开始扣除法力值时，低于此值将停止当前动作。适用于启用「魔力之体」特性时。</t>
   </si>
 </sst>
 </file>
@@ -173,7 +644,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -197,13 +668,7 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Microsoft YaHei"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Microsoft YaHei"/>
+      <name val="Noto Sans SC"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -249,7 +714,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -258,11 +723,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -389,18 +858,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+      <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="32.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="68.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="55.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="48.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="68.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="55.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="48.59"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="5" style="1" width="11.53"/>
   </cols>
   <sheetData>
@@ -408,13 +877,13 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -422,13 +891,13 @@
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -436,13 +905,13 @@
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>11</v>
       </c>
     </row>
@@ -450,13 +919,13 @@
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>15</v>
       </c>
     </row>
@@ -464,13 +933,13 @@
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>19</v>
       </c>
     </row>
@@ -478,13 +947,13 @@
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="3" t="s">
         <v>23</v>
       </c>
     </row>
@@ -492,13 +961,13 @@
       <c r="A7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="3" t="s">
         <v>27</v>
       </c>
     </row>
@@ -506,13 +975,13 @@
       <c r="A8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="3" t="s">
         <v>31</v>
       </c>
     </row>
@@ -520,7 +989,7 @@
       <c r="A9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -534,13 +1003,13 @@
       <c r="A10" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="3" t="s">
         <v>39</v>
       </c>
     </row>
@@ -548,13 +1017,13 @@
       <c r="A11" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="3" t="s">
         <v>43</v>
       </c>
     </row>
@@ -562,14 +1031,168 @@
       <c r="A12" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="3" t="s">
         <v>47</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" s="4" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>